<commit_message>
Add sample_name_prefix argument to data loading
Add a sample_name_prefix argument the accucor data loading command that
adds the prefix before looking up the sample name in the database.

Resolves #184
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" state="visible" r:id="rId2"/>
@@ -337,7 +337,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t xml:space="preserve">Animal ID</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t xml:space="preserve">Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREFIX_newsample</t>
   </si>
   <si>
     <t xml:space="preserve">Treatment Description</t>
@@ -528,6 +531,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -557,6 +561,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -671,11 +676,11 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -770,13 +775,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD16"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1112,10 +1117,30 @@
         <v>971</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>971</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1135,14 +1160,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1172,7 +1197,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add sample_name_prefix argument to data loading (#187)
* Add sample_name_prefix argument to data loading

Add a sample_name_prefix argument the accucor data loading command that
adds the prefix before looking up the sample name in the database.

Resolves #184
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" state="visible" r:id="rId2"/>
@@ -337,7 +337,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t xml:space="preserve">Animal ID</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t xml:space="preserve">Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREFIX_newsample</t>
   </si>
   <si>
     <t xml:space="preserve">Treatment Description</t>
@@ -528,6 +531,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -557,6 +561,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -671,11 +676,11 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -770,13 +775,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD16"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1112,10 +1117,30 @@
         <v>971</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>971</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1135,14 +1160,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1172,7 +1197,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add initial tissue fixtures
* Create a fixture that contains the valid tissue types
* Add an optional tissue description field
* Require tissue be found when loading samples
* Load tissue fixtures before running tests

Addresses part of #191
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -426,19 +426,19 @@
     <t xml:space="preserve">Br-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Brain</t>
+    <t xml:space="preserve">brain</t>
   </si>
   <si>
     <t xml:space="preserve">Dia-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Diaphragm</t>
+    <t xml:space="preserve">diaph</t>
   </si>
   <si>
     <t xml:space="preserve">gas-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Gastrocnemius</t>
+    <t xml:space="preserve">gast</t>
   </si>
   <si>
     <t xml:space="preserve">gWAT-xz971</t>
@@ -450,55 +450,55 @@
     <t xml:space="preserve">H-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Heart</t>
+    <t xml:space="preserve">heart</t>
   </si>
   <si>
     <t xml:space="preserve">Kid-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Kidney</t>
+    <t xml:space="preserve">kidney</t>
   </si>
   <si>
     <t xml:space="preserve">Liv-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Liver</t>
+    <t xml:space="preserve">liver</t>
   </si>
   <si>
     <t xml:space="preserve">Lu-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Lung</t>
+    <t xml:space="preserve">lung</t>
   </si>
   <si>
     <t xml:space="preserve">Pc-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Pancreas</t>
+    <t xml:space="preserve">pancreas</t>
   </si>
   <si>
     <t xml:space="preserve">Q-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Quad</t>
+    <t xml:space="preserve">quad</t>
   </si>
   <si>
     <t xml:space="preserve">SI-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Small Intestine</t>
+    <t xml:space="preserve">SmIn</t>
   </si>
   <si>
     <t xml:space="preserve">Sol-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Soleus</t>
+    <t xml:space="preserve">soleus</t>
   </si>
   <si>
     <t xml:space="preserve">Sp-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Spleen</t>
+    <t xml:space="preserve">spleen</t>
   </si>
   <si>
     <t xml:space="preserve">serum-xz971</t>
@@ -507,7 +507,7 @@
     <t xml:space="preserve">11/19/20</t>
   </si>
   <si>
-    <t xml:space="preserve">Serum</t>
+    <t xml:space="preserve">serum</t>
   </si>
   <si>
     <t xml:space="preserve">PREFIX_newsample</t>
@@ -680,7 +680,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -778,10 +778,10 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1160,7 +1160,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
Add initial tissue fixtures (#192)
* Add initial tissue fixtures

* Create a fixture that contains the valid tissue types
* Add an optional tissue description field
* Require tissue be found when loading samples
* Load tissue fixtures before running tests

Addresses part of #191

* Standardized tissue names in examples

* Updated tissue names
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -420,85 +420,85 @@
     <t xml:space="preserve">Xianfeng Zhang</t>
   </si>
   <si>
-    <t xml:space="preserve">BAT</t>
+    <t xml:space="preserve">brown_adipose_tissue</t>
   </si>
   <si>
     <t xml:space="preserve">Br-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Brain</t>
+    <t xml:space="preserve">brain</t>
   </si>
   <si>
     <t xml:space="preserve">Dia-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Diaphragm</t>
+    <t xml:space="preserve">diaphragm</t>
   </si>
   <si>
     <t xml:space="preserve">gas-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Gastrocnemius</t>
+    <t xml:space="preserve">gastrocnemius</t>
   </si>
   <si>
     <t xml:space="preserve">gWAT-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">gWAT</t>
+    <t xml:space="preserve">white_adipose_tissue_gonadal</t>
   </si>
   <si>
     <t xml:space="preserve">H-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Heart</t>
+    <t xml:space="preserve">heart</t>
   </si>
   <si>
     <t xml:space="preserve">Kid-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Kidney</t>
+    <t xml:space="preserve">kidney</t>
   </si>
   <si>
     <t xml:space="preserve">Liv-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Liver</t>
+    <t xml:space="preserve">liver</t>
   </si>
   <si>
     <t xml:space="preserve">Lu-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Lung</t>
+    <t xml:space="preserve">lung</t>
   </si>
   <si>
     <t xml:space="preserve">Pc-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Pancreas</t>
+    <t xml:space="preserve">pancreas</t>
   </si>
   <si>
     <t xml:space="preserve">Q-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Quad</t>
+    <t xml:space="preserve">quadricep</t>
   </si>
   <si>
     <t xml:space="preserve">SI-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Small Intestine</t>
+    <t xml:space="preserve">small_intestine</t>
   </si>
   <si>
     <t xml:space="preserve">Sol-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Soleus</t>
+    <t xml:space="preserve">soleus</t>
   </si>
   <si>
     <t xml:space="preserve">Sp-xz971</t>
   </si>
   <si>
-    <t xml:space="preserve">Spleen</t>
+    <t xml:space="preserve">spleen</t>
   </si>
   <si>
     <t xml:space="preserve">serum-xz971</t>
@@ -507,7 +507,7 @@
     <t xml:space="preserve">11/19/20</t>
   </si>
   <si>
-    <t xml:space="preserve">Serum</t>
+    <t xml:space="preserve">serum_plasma_unspecified_location</t>
   </si>
   <si>
     <t xml:space="preserve">PREFIX_newsample</t>
@@ -680,7 +680,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -778,10 +778,13 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.75"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1160,7 +1163,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
Fix name in Excel sheet
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -417,7 +417,7 @@
     <t xml:space="preserve">2020-11-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Xianfeng Zhang</t>
+    <t xml:space="preserve">Xianfeng Zeng</t>
   </si>
   <si>
     <t xml:space="preserve">brown_adipose_tissue</t>
@@ -677,10 +677,10 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C2:C17 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -778,10 +778,10 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="C2:C17 D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.75"/>
   </cols>
@@ -1160,10 +1160,10 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C17 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
Change Xianfeng Zhang to Xianfeng Zeng (#288)
* Change Xianfeng Zhang to Xianfeng Zeng

Resolves #274
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -417,7 +417,7 @@
     <t xml:space="preserve">2020-11-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Xianfeng Zhang</t>
+    <t xml:space="preserve">Xianfeng Zeng</t>
   </si>
   <si>
     <t xml:space="preserve">brown_adipose_tissue</t>
@@ -677,10 +677,10 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C2:C17 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -778,10 +778,10 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="C2:C17 D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.75"/>
   </cols>
@@ -1160,10 +1160,10 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C17 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
Fixed example data load in the ci test yaml.
- Fixed data for StudyLoadingTests and updated the multi tag associated with it.
- Typo fix.

Files checked in: DataRepo/example_data/obob_sample_table.tsv DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx DataRepo/models/animal.py DataRepo/tests/test_models.py
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/small_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF2C30A-3386-AB44-86C4-8A6253AB33CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD66ED2-C7D6-3E4A-A615-17848634306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19540" yWindow="14620" windowWidth="29900" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="4340" windowWidth="29900" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -166,10 +166,17 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>An identifier for the "experiment", which is typically a collection of mice similar infusion parameters. this is loosely defined based on the person who did the infusions. Here, there is a consistant format: two initials for the lab member who did the infusion and then a number (date?)
-	-Lance Parsons</t>
+          <t xml:space="preserve">An identifier for the "experiment", which is typically a collection of mice similar infusion parameters. this is loosely defined based on the person who did the infusions. Here, there is a consistant format: two initials for the lab member who did the infusion and then a number (date?)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">	-Lance Parsons</t>
         </r>
       </text>
     </comment>
@@ -180,10 +187,17 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>A long form description for the study which may include the experimental design process, citations, and other relevant details
-	-Lance Parsons</t>
+          <t xml:space="preserve">A long form description for the study which may include the experimental design process, citations, and other relevant details
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">	-Lance Parsons</t>
         </r>
       </text>
     </comment>
@@ -417,12 +431,6 @@
   </si>
   <si>
     <t>Animal Treatment</t>
-  </si>
-  <si>
-    <t>Study Name</t>
-  </si>
-  <si>
-    <t>Study Description</t>
   </si>
   <si>
     <t>Sample Name</t>
@@ -788,6 +796,12 @@
   <si>
     <t>PREFIX_newsample</t>
   </si>
+  <si>
+    <t>Experiment Name</t>
+  </si>
+  <si>
+    <t>Experiment Description</t>
+  </si>
 </sst>
 </file>
 
@@ -796,7 +810,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -872,6 +886,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1164,7 +1183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1206,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
@@ -1217,13 +1236,13 @@
         <v>971</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="23">
         <v>26.3</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" s="23">
         <v>23.2</v>
@@ -1232,16 +1251,16 @@
         <v>0.11</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="23" t="s">
-        <v>97</v>
-      </c>
       <c r="J2" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -4277,19 +4296,19 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -4311,16 +4330,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="23">
         <v>150</v>
@@ -4341,16 +4360,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23">
         <v>150</v>
@@ -4371,16 +4390,16 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="23">
         <v>150</v>
@@ -4401,16 +4420,16 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="23">
         <v>150</v>
@@ -4431,16 +4450,16 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="23">
         <v>150</v>
@@ -4461,16 +4480,16 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="23">
         <v>150</v>
@@ -4491,16 +4510,16 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="23">
         <v>150</v>
@@ -4521,16 +4540,16 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="23">
         <v>150</v>
@@ -4551,16 +4570,16 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="23">
         <v>150</v>
@@ -4581,16 +4600,16 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="23">
         <v>150</v>
@@ -4611,16 +4630,16 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12" s="23">
         <v>150</v>
@@ -4641,16 +4660,16 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="23">
         <v>150</v>
@@ -4671,16 +4690,16 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="23">
         <v>150</v>
@@ -4701,16 +4720,16 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E15" s="23">
         <v>150</v>
@@ -4731,16 +4750,16 @@
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="23">
         <v>150</v>
@@ -4761,16 +4780,16 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="23">
         <v>150</v>
@@ -22538,7 +22557,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -22567,10 +22586,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -22600,10 +22619,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="7"/>
@@ -22629,297 +22648,297 @@
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="15">
       <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="11" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" ht="15">
+      <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="11" t="s">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:26" ht="15">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:26">
-      <c r="A5" s="11" t="s">
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:26">
-      <c r="A6" s="15" t="s">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:26" ht="15">
+      <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:26">
-      <c r="A7" s="11" t="s">
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:26" ht="15">
+      <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:26">
-      <c r="A8" s="11" t="s">
+      <c r="B9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:26" ht="15">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="A9" s="11" t="s">
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:26" ht="15">
+      <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:26">
-      <c r="A10" s="11" t="s">
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:26" ht="15">
+      <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:26">
-      <c r="A11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="11" t="s">
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:26" ht="15">
+      <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="11" t="s">
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:26" ht="15">
+      <c r="A14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A17" s="15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B17" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A17" s="15" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A21" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B24" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A26" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B27" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A28" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A29" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A30" s="11" t="s">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A31" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A31" s="11" t="s">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A32" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B33" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A34" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="B34" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A35" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -22939,7 +22958,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
@@ -22971,76 +22990,76 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A5" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="19" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="19" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="19" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" ht="18">
       <c r="A17" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -23070,22 +23089,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Previous data file changes broke some test class setups, so I revised the solution.
Files checked in: .github/workflows/tracebase-tests.yml DataRepo/example_data/obob_sample_table.tsv DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/small_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD66ED2-C7D6-3E4A-A615-17848634306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E948BB0-9010-2046-93C6-B9F01109A63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="4340" windowWidth="29900" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,17 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Unique identifier for the animal (mouse) the sample was collected from. MUST match the Animal ID in the Animal Table.
-	-Lance Parsons</t>
+          <t xml:space="preserve">Unique identifier for the animal (mouse) the sample was collected from. MUST match the Animal ID in the Animal Table.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">	-Lance Parsons</t>
         </r>
       </text>
     </comment>
@@ -433,6 +440,12 @@
     <t>Animal Treatment</t>
   </si>
   <si>
+    <t>Study Name</t>
+  </si>
+  <si>
+    <t>Study Description</t>
+  </si>
+  <si>
     <t>Sample Name</t>
   </si>
   <si>
@@ -795,12 +808,6 @@
   </si>
   <si>
     <t>PREFIX_newsample</t>
-  </si>
-  <si>
-    <t>Experiment Name</t>
-  </si>
-  <si>
-    <t>Experiment Description</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1190,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1225,10 +1232,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
@@ -1236,13 +1243,13 @@
         <v>971</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="23">
         <v>26.3</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" s="23">
         <v>23.2</v>
@@ -1251,16 +1258,16 @@
         <v>0.11</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -4296,19 +4303,19 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -4330,16 +4337,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="23">
         <v>150</v>
@@ -4360,16 +4367,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>98</v>
-      </c>
       <c r="C3" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="23">
         <v>150</v>
@@ -4390,16 +4397,16 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>99</v>
-      </c>
       <c r="D4" s="23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="23">
         <v>150</v>
@@ -4420,16 +4427,16 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="23">
         <v>150</v>
@@ -4450,16 +4457,16 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="23">
         <v>150</v>
@@ -4480,16 +4487,16 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E7" s="23">
         <v>150</v>
@@ -4510,16 +4517,16 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="23">
         <v>150</v>
@@ -4540,16 +4547,16 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" s="23">
         <v>150</v>
@@ -4570,16 +4577,16 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="23" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="23">
         <v>150</v>
@@ -4600,16 +4607,16 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11" s="23">
         <v>150</v>
@@ -4630,16 +4637,16 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12" s="23">
         <v>150</v>
@@ -4660,16 +4667,16 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E13" s="23">
         <v>150</v>
@@ -4690,16 +4697,16 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="23">
         <v>150</v>
@@ -4720,16 +4727,16 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E15" s="23">
         <v>150</v>
@@ -4750,16 +4757,16 @@
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E16" s="23">
         <v>150</v>
@@ -4780,16 +4787,16 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17" s="23">
         <v>150</v>
@@ -22557,7 +22564,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -22586,10 +22593,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -22619,10 +22626,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="7"/>
@@ -22650,295 +22657,295 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:26" ht="15">
       <c r="A4" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:26" ht="15">
       <c r="A5" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:26" ht="15">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="15">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:26" ht="15">
       <c r="A8" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:26" ht="15">
       <c r="A9" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:26" ht="15">
       <c r="A10" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:26" ht="15">
       <c r="A11" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:26" ht="15">
       <c r="A12" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:26" ht="15">
       <c r="A13" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:26" ht="15">
       <c r="A14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -22990,68 +22997,68 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
@@ -23059,7 +23066,7 @@
     </row>
     <row r="17" spans="1:26" ht="18">
       <c r="A17" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -23089,22 +23096,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Removal of auto-loaded animal treatments
load_study now knows about protocols_loader
load_protocols can handle tsv or xlxs animals template
Fixed a subset of easily interpretable broken-tests
Forgotten modified files from previous commit
Many more broken tests likely remain
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/small_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcmatese/dev/tracebase/DataRepo/example_data/small_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E948BB0-9010-2046-93C6-B9F01109A63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0781DF80-725F-314E-A46A-292FFFD541A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="4340" windowWidth="29900" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="5120" windowWidth="29900" windowHeight="12800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -335,10 +335,17 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>A thorough description of an animal treatment protocol. This will be useful for searching and filtering, so use standard terms and be as complete as possible.
-	-Lance Parsons</t>
+          <t xml:space="preserve">A thorough description of an animal treatment protocol. This will be useful for searching and filtering, so use standard terms and be as complete as possible.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">	-Lance Parsons</t>
         </r>
       </text>
     </comment>
@@ -414,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
   <si>
     <t>Animal ID</t>
   </si>
@@ -809,6 +816,9 @@
   <si>
     <t>PREFIX_newsample</t>
   </si>
+  <si>
+    <t>ob/ob homozygouse mice were fasted</t>
+  </si>
 </sst>
 </file>
 
@@ -1188,9 +1198,9 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -22546,9 +22556,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -22597,6 +22607,14 @@
       </c>
       <c r="B2" s="11" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusion of protocols in the user data validation view.
Note, this changes the treatment of protocol loads from being like tissues & compounds to being like everything else.
It adds every error to the error output when verbosity is greater than 1.
It copies data from the default database to the validation database any time a file is validated and everything is cleaned out at the end.

Files checked in: DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx DataRepo/utils/protocols_loader.py DataRepo/views/loading/validation.py
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcmatese/dev/tracebase/DataRepo/example_data/small_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/small_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0781DF80-725F-314E-A46A-292FFFD541A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EC9D00-BC86-984D-A0E7-8D8D048EAAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="5120" windowWidth="29900" windowHeight="12800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>no treatment</t>
   </si>
   <si>
-    <t>No treatment was applied to the animal.  Animal was maintained on normal diet (LabDiet #5053 "Maintenance"), housed at room temperature with a normal light cycle.</t>
-  </si>
-  <si>
     <t>TraceBase Tissue Name</t>
   </si>
   <si>
@@ -818,6 +815,9 @@
   </si>
   <si>
     <t>ob/ob homozygouse mice were fasted</t>
+  </si>
+  <si>
+    <t>No manipulation besides what is already described in other fields.</t>
   </si>
 </sst>
 </file>
@@ -1253,13 +1253,13 @@
         <v>971</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="23">
         <v>26.3</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="23">
         <v>23.2</v>
@@ -1268,16 +1268,16 @@
         <v>0.11</v>
       </c>
       <c r="G2" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="23" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -4347,16 +4347,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="23">
         <v>150</v>
@@ -4377,16 +4377,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="23">
         <v>150</v>
@@ -4407,16 +4407,16 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D4" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="23">
         <v>150</v>
@@ -4437,16 +4437,16 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D5" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="23">
         <v>150</v>
@@ -4467,16 +4467,16 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="23">
         <v>150</v>
@@ -4497,16 +4497,16 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D7" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="23">
         <v>150</v>
@@ -4527,16 +4527,16 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="23">
         <v>150</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D9" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="23">
         <v>150</v>
@@ -4587,16 +4587,16 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D10" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="23">
         <v>150</v>
@@ -4617,16 +4617,16 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="23">
         <v>150</v>
@@ -4647,16 +4647,16 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D12" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="23">
         <v>150</v>
@@ -4677,16 +4677,16 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D13" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="23">
         <v>150</v>
@@ -4707,16 +4707,16 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D14" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="23">
         <v>150</v>
@@ -4737,16 +4737,16 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D15" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="23">
         <v>150</v>
@@ -4767,16 +4767,16 @@
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>116</v>
-      </c>
       <c r="C16" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="23">
         <v>150</v>
@@ -4797,16 +4797,16 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="23">
         <v>150</v>
@@ -22560,7 +22560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -22606,15 +22606,15 @@
         <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -22644,10 +22644,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="7"/>
@@ -22675,295 +22675,295 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:26" ht="15">
-      <c r="A3" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" ht="15">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:26" ht="15">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:26" ht="15">
-      <c r="A6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:26" ht="15">
+      <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:26" ht="15">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:26" ht="15">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:26" ht="15">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:26" ht="15">
-      <c r="A9" s="11" t="s">
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:26" ht="15">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:26" ht="15">
-      <c r="A10" s="11" t="s">
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:26" ht="15">
+      <c r="A11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:26" ht="15">
-      <c r="A11" s="11" t="s">
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:26" ht="15">
+      <c r="A12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:26" ht="15">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:26" ht="15">
+      <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:26" ht="15">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:26" ht="15">
+      <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:26" ht="15">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="11" t="s">
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A17" s="15" t="s">
+      <c r="B17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="11" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
+      <c r="B18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="11" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="11" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A21" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A22" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="11" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A23" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="15" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="B24" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A26" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="11" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="B27" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A29" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A30" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="11" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A31" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A31" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="11" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A32" s="11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="15" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B34" s="15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="11" t="s">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -23015,76 +23015,76 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="19" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A5" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="19" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="19" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="19" t="s">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="18">
       <c r="A17" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -23114,22 +23114,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A20" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>